<commit_message>
Update the estimation times #pair[rmc209, ebb35]
</commit_message>
<xml_diff>
--- a/sprint6EstimatedTimes.xlsx
+++ b/sprint6EstimatedTimes.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucliveac-my.sharepoint.com/personal/rmc209_uclive_ac_nz/Documents/SENG302/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebek\OneDrive - University of Canterbury\SENG302\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10430196-5930-4A8F-8551-13C767A65B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="316" documentId="8_{10430196-5930-4A8F-8551-13C767A65B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FC3EDCF-298B-449C-AE3E-7E232E8DA04A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595"/>
+    <workbookView xWindow="105" yWindow="368" windowWidth="22305" windowHeight="7747" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agilefant Timesheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="132">
   <si>
     <t>Story Id</t>
   </si>
@@ -34,21 +44,12 @@
     <t>Task</t>
   </si>
   <si>
-    <t>4154</t>
-  </si>
-  <si>
     <t>Planning out solving our Technical Debt problem</t>
   </si>
   <si>
-    <t>4319</t>
-  </si>
-  <si>
     <t>Sprint Planning</t>
   </si>
   <si>
-    <t>4596</t>
-  </si>
-  <si>
     <t>Standup</t>
   </si>
   <si>
@@ -344,16 +345,97 @@
   </si>
   <si>
     <t>Actual Effort</t>
+  </si>
+  <si>
+    <t>Add activity to the search for drop down</t>
+  </si>
+  <si>
+    <t>Implement error handling on the front end</t>
+  </si>
+  <si>
+    <t>Add MapViewer.vue component to ViewProfile.vue page.</t>
+  </si>
+  <si>
+    <t>U39 - Activity Geolocation</t>
+  </si>
+  <si>
+    <t>Modify the activity class to link to one location object</t>
+  </si>
+  <si>
+    <t>Modify the activityValidator to check Location objects within activities. BACK-END</t>
+  </si>
+  <si>
+    <t>Modify ActivityResponse payload to include location. BACK-END</t>
+  </si>
+  <si>
+    <t>Implement the use of LocationIO within ActivityForm.vue for creating and editing activities</t>
+  </si>
+  <si>
+    <t>Add my location and activity location pins to the LocationIO component (give to its prop)</t>
+  </si>
+  <si>
+    <t>U42 Pins - (Modified ACs)</t>
+  </si>
+  <si>
+    <t>Create pin class</t>
+  </si>
+  <si>
+    <t>Create ActivityService for converting List Activity to List Pin</t>
+  </si>
+  <si>
+    <t>Create endpoint for getting pin information (in blocks)</t>
+  </si>
+  <si>
+    <t>Add map pane to all activities page (Using MapViewer.vue component)</t>
+  </si>
+  <si>
+    <t>U34 - Activities near me</t>
+  </si>
+  <si>
+    <t>Set map to load centered on your location</t>
+  </si>
+  <si>
+    <t>Add sorting to ActivityService for sorting by distance to a location</t>
+  </si>
+  <si>
+    <t>Add pins on the map given their longitube/latitude value (MapViewer.vue)</t>
+  </si>
+  <si>
+    <t>Hover window for pins</t>
+  </si>
+  <si>
+    <t>Add endpoint to ActivityController for searching by location</t>
+  </si>
+  <si>
+    <t>Link pins to go to activity detail page when clicked</t>
+  </si>
+  <si>
+    <t>Add "Location" option to search by dropdown</t>
+  </si>
+  <si>
+    <t>TOTALS</t>
+  </si>
+  <si>
+    <t>Add LocationIO.vue to ActivitySearch.vue for inputing location search field for activity</t>
+  </si>
+  <si>
+    <t>Add Location Details to User Payload. Response</t>
+  </si>
+  <si>
+    <t>Add my location (public and/or private) pins to the LocationIO component (give to its prop)</t>
+  </si>
+  <si>
+    <t>Manually moving a pin to the location you want, will enter an address in the textbox.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="dd\.mm\.yyyy\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -363,13 +445,42 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -384,12 +495,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -705,791 +845,1495 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.3984375" customWidth="1"/>
-    <col min="2" max="2" width="33.86328125" customWidth="1"/>
-    <col min="3" max="3" width="7.796875" customWidth="1"/>
-    <col min="4" max="4" width="104.796875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="16.73046875" customWidth="1"/>
+    <col min="1" max="1" width="8.3984375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="33.86328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="104.796875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.73046875" style="5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="19.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="10">
+        <v>4596</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="11">
+        <v>33.75</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="10">
+        <v>4319</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="11">
+        <v>36</v>
+      </c>
+      <c r="F3" s="11">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="10">
+        <v>4154</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E4" s="11">
+        <v>13.5</v>
+      </c>
+      <c r="F4" s="11">
+        <v>27.3</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" s="15">
+        <v>2</v>
+      </c>
+      <c r="F6" s="15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" s="15">
+        <v>2</v>
+      </c>
+      <c r="F7" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" s="15">
+        <v>2</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" s="15">
+        <v>2</v>
+      </c>
+      <c r="F10" s="15">
+        <v>18.8</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" s="15">
+        <v>2</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="D12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.5</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
+      <c r="D13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2.5</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>3.3</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="5">
+        <v>3</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3.3</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.2</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18">
+        <v>422</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="14">
+        <v>4326</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="15">
+        <v>0</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E19" s="15">
+        <v>2</v>
+      </c>
+      <c r="F19" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
+    </row>
+    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E20" s="15">
+        <v>3</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1.7</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E21" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E22" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D23" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E23" s="15">
+        <v>3</v>
+      </c>
+      <c r="F23" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D24" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E24" s="15">
+        <v>3</v>
+      </c>
+      <c r="F24" s="15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D25" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E25" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F25" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D26" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E26" s="15">
+        <v>3</v>
+      </c>
+      <c r="F26" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E27" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="15">
+        <v>1</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D28" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E28" s="15">
+        <v>3</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D29" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E29" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17"/>
+    </row>
+    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D30" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E30" s="15">
+        <v>3</v>
+      </c>
+      <c r="F30" s="15">
+        <v>5.9</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="14">
+        <v>422</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="14">
+        <v>4359</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="15">
+        <v>1</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D32" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E32" s="15">
+        <v>3</v>
+      </c>
+      <c r="F32" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="G32" s="16"/>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B33" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C33" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="D33" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" t="s">
-        <v>73</v>
+      <c r="E33" s="5">
+        <v>2</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="A34" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" t="s">
-        <v>75</v>
+      <c r="D34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1.5</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" t="s">
-        <v>77</v>
+      <c r="A35" s="6">
+        <v>420</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="6">
+        <v>4591</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" t="s">
-        <v>79</v>
+      <c r="A36" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="5">
+        <v>1.5</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" t="s">
-        <v>81</v>
+      <c r="A37" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1.3</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" t="s">
-        <v>83</v>
+      <c r="A38" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="5">
+        <v>3</v>
+      </c>
+      <c r="F38" s="5">
+        <v>4.5</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" t="s">
-        <v>85</v>
+      <c r="A39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="5">
+        <v>3</v>
+      </c>
+      <c r="F39" s="5">
+        <v>10.4</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" t="s">
-        <v>86</v>
-      </c>
-      <c r="D40" t="s">
-        <v>87</v>
+      <c r="A40" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="5">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0.8</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" t="s">
-        <v>89</v>
+      <c r="A41" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0.5</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" t="s">
-        <v>93</v>
+      <c r="A42" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1.2</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" t="s">
-        <v>95</v>
+      <c r="A43" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="5">
+        <v>2</v>
+      </c>
+      <c r="F43" s="5">
+        <v>1.8</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" t="s">
-        <v>97</v>
+      <c r="A44" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="5">
+        <v>2</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0.5</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="45" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F45" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="17"/>
+    </row>
+    <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B45" t="s">
+      <c r="E46" s="15">
+        <v>3</v>
+      </c>
+      <c r="F46" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="17"/>
+    </row>
+    <row r="47" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="15">
+        <v>3</v>
+      </c>
+      <c r="F47" s="15">
+        <v>1.6</v>
+      </c>
+      <c r="G47" s="16"/>
+      <c r="H47" s="17"/>
+    </row>
+    <row r="48" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="15">
+        <v>3</v>
+      </c>
+      <c r="F48" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="17"/>
+    </row>
+    <row r="49" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F49" s="15">
+        <v>1</v>
+      </c>
+      <c r="G49" s="16"/>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C45" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" t="s">
-        <v>99</v>
-      </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" t="s">
-        <v>101</v>
-      </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>90</v>
-      </c>
-      <c r="B47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" t="s">
-        <v>103</v>
-      </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="2"/>
+      <c r="D50" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F50" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="14">
+        <v>4589</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F51" s="15"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="17"/>
+    </row>
+    <row r="52" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="14">
+        <v>4793</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" s="15">
+        <v>2</v>
+      </c>
+      <c r="F52" s="15"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="17"/>
+    </row>
+    <row r="53" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" s="14">
+        <v>4730</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="15">
+        <v>6</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="17"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="6">
+        <v>421</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="6">
+        <v>4712</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="6">
+        <v>421</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="6">
+        <v>4718</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E55" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="6">
+        <v>421</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="6">
+        <v>4713</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="6">
+        <v>421</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="6">
+        <v>4715</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E57" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="6">
+        <v>421</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="6">
+        <v>4721</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="14">
+        <v>450</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="14">
+        <v>4735</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="15">
+        <v>2</v>
+      </c>
+      <c r="F59" s="15"/>
+    </row>
+    <row r="60" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="14">
+        <v>450</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="14">
+        <v>4239</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E60" s="15">
+        <v>3</v>
+      </c>
+      <c r="F60" s="15"/>
+    </row>
+    <row r="61" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="14">
+        <v>450</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="14">
+        <v>4734</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" s="15">
+        <v>3</v>
+      </c>
+      <c r="F61" s="15"/>
+    </row>
+    <row r="62" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="14">
+        <v>450</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="14">
+        <v>4720</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" s="15">
+        <v>1</v>
+      </c>
+      <c r="F62" s="15"/>
+    </row>
+    <row r="63" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="14">
+        <v>450</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="14">
+        <v>4731</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F63" s="15"/>
+    </row>
+    <row r="64" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="14">
+        <v>450</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="14">
+        <v>4585</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E64" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F64" s="15"/>
+    </row>
+    <row r="65" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="14">
+        <v>450</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="14">
+        <v>4733</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E65" s="15">
+        <v>3</v>
+      </c>
+      <c r="F65" s="15"/>
+    </row>
+    <row r="66" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="14">
+        <v>450</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="14">
+        <v>4732</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E66" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F66" s="15"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="6">
+        <v>451</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="6">
+        <v>4740</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="6">
+        <v>451</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="6">
+        <v>4737</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E68" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" s="6">
+        <v>451</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" s="6">
+        <v>4738</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E69" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="6">
+        <v>451</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="6">
+        <v>4736</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E70" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+    </row>
+    <row r="76" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B76" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="5">
+        <f>SUM(E5:E70)</f>
+        <v>140.5</v>
+      </c>
+      <c r="F76" s="5">
+        <f>SUM(F5:F70)</f>
+        <v>101.50000000000001</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="B76:D76"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100659A167D4CC5EC438DE9848E11CBEA3F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b214d0967801b5c4681ff9774ab7b4fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7a535a6-dfd7-4199-be2a-842d35677326" xmlns:ns4="b1af40a2-86c1-4bae-9fd5-ad1d161ccb8d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ba29263248737a5ec68c1b9165b2e49" ns3:_="" ns4:_="">
     <xsd:import namespace="b7a535a6-dfd7-4199-be2a-842d35677326"/>
@@ -1712,7 +2556,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1721,13 +2565,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11FB2DEE-0B14-4095-888E-5BA73ECE0B4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b7a535a6-dfd7-4199-be2a-842d35677326"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b1af40a2-86c1-4bae-9fd5-ad1d161ccb8d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB27589-92E7-461D-B68C-D866F96320FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1746,27 +2601,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{631E28D5-CD26-42A3-901C-27469E6CABF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11FB2DEE-0B14-4095-888E-5BA73ECE0B4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b7a535a6-dfd7-4199-be2a-842d35677326"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b1af40a2-86c1-4bae-9fd5-ad1d161ccb8d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating spreadsheet with new Task 4952
</commit_message>
<xml_diff>
--- a/sprint6EstimatedTimes.xlsx
+++ b/sprint6EstimatedTimes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebek\OneDrive - University of Canterbury\SENG302\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\games\Documents\2020\SENG302\SENG302 Project\team-600\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="8_{10430196-5930-4A8F-8551-13C767A65B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FC3EDCF-298B-449C-AE3E-7E232E8DA04A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1E1B6-7865-461E-BB0F-F3E0698B5857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="368" windowWidth="22305" windowHeight="7747" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agilefant Timesheet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="133">
   <si>
     <t>Story Id</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>Manually moving a pin to the location you want, will enter an address in the textbox.</t>
+  </si>
+  <si>
+    <t>Fix display issues on Front- End UI</t>
   </si>
 </sst>
 </file>
@@ -846,26 +849,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.3984375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="33.86328125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="7.796875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="104.796875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="104.77734375" style="6" customWidth="1"/>
     <col min="5" max="5" width="16" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.73046875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="19.796875" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -887,7 +890,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>101</v>
       </c>
@@ -907,7 +910,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>101</v>
       </c>
@@ -929,7 +932,7 @@
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>101</v>
       </c>
@@ -951,7 +954,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>101</v>
       </c>
@@ -973,7 +976,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="17"/>
     </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>101</v>
       </c>
@@ -995,7 +998,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>101</v>
       </c>
@@ -1017,7 +1020,7 @@
       <c r="G7" s="16"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>101</v>
       </c>
@@ -1039,7 +1042,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
     </row>
-    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>101</v>
       </c>
@@ -1061,7 +1064,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>101</v>
       </c>
@@ -1083,7 +1086,7 @@
       <c r="G10" s="16"/>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>101</v>
       </c>
@@ -1105,7 +1108,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1127,7 +1130,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1152,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -1171,7 +1174,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -1190,7 +1193,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1215,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -1234,7 +1237,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>422</v>
       </c>
@@ -1256,7 +1259,7 @@
       <c r="G18" s="16"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>35</v>
       </c>
@@ -1278,7 +1281,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>35</v>
       </c>
@@ -1300,7 +1303,7 @@
       <c r="G20" s="16"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -1320,7 +1323,7 @@
       <c r="G21" s="16"/>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>35</v>
       </c>
@@ -1340,7 +1343,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>35</v>
       </c>
@@ -1362,7 +1365,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1387,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>35</v>
       </c>
@@ -1406,7 +1409,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="17"/>
     </row>
-    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>35</v>
       </c>
@@ -1428,7 +1431,7 @@
       <c r="G26" s="16"/>
       <c r="H26" s="17"/>
     </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>35</v>
       </c>
@@ -1450,7 +1453,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>35</v>
       </c>
@@ -1470,7 +1473,7 @@
       <c r="G28" s="16"/>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
@@ -1490,7 +1493,7 @@
       <c r="G29" s="16"/>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>35</v>
       </c>
@@ -1512,7 +1515,7 @@
       <c r="G30" s="16"/>
       <c r="H30" s="17"/>
     </row>
-    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>422</v>
       </c>
@@ -1532,7 +1535,7 @@
       <c r="G31" s="16"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>35</v>
       </c>
@@ -1554,26 +1557,27 @@
       <c r="G32" s="16"/>
       <c r="H32" s="17"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="5">
+    <row r="33" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>422</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="14">
+        <v>4952</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="15">
         <v>2</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>63</v>
       </c>
@@ -1581,59 +1585,59 @@
         <v>64</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E34" s="5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
-        <v>420</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="6">
-        <v>4591</v>
+      <c r="C35" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="E35" s="5">
         <v>1.5</v>
       </c>
-      <c r="F35" s="5">
-        <v>0</v>
-      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
-        <v>63</v>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>420</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>69</v>
+      <c r="C36" s="6">
+        <v>4591</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="E36" s="5">
         <v>1.5</v>
       </c>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
@@ -1641,21 +1645,18 @@
         <v>64</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E37" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F37" s="5">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>63</v>
       </c>
@@ -1663,21 +1664,21 @@
         <v>64</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E38" s="5">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F38" s="5">
-        <v>4.5</v>
+        <v>1.3</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>63</v>
       </c>
@@ -1685,21 +1686,21 @@
         <v>64</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E39" s="5">
         <v>3</v>
       </c>
       <c r="F39" s="5">
-        <v>10.4</v>
+        <v>4.5</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>63</v>
       </c>
@@ -1707,21 +1708,21 @@
         <v>64</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E40" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F40" s="5">
-        <v>0.8</v>
+        <v>10.4</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>63</v>
       </c>
@@ -1729,18 +1730,21 @@
         <v>64</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E41" s="5">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.8</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>63</v>
       </c>
@@ -1748,21 +1752,18 @@
         <v>64</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E42" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F42" s="5">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>63</v>
       </c>
@@ -1770,21 +1771,21 @@
         <v>64</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E43" s="5">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F43" s="5">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>63</v>
       </c>
@@ -1792,43 +1793,43 @@
         <v>64</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
       </c>
       <c r="F44" s="5">
-        <v>0.5</v>
+        <v>1.8</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="F45" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G45" s="16"/>
-      <c r="H45" s="17"/>
-    </row>
-    <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="5">
+        <v>2</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>87</v>
       </c>
@@ -1836,21 +1837,21 @@
         <v>88</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E46" s="15">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F46" s="15">
-        <v>2.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>87</v>
       </c>
@@ -1858,21 +1859,21 @@
         <v>88</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E47" s="15">
         <v>3</v>
       </c>
       <c r="F47" s="15">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="17"/>
     </row>
-    <row r="48" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>87</v>
       </c>
@@ -1880,21 +1881,21 @@
         <v>88</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E48" s="15">
         <v>3</v>
       </c>
       <c r="F48" s="15">
-        <v>2.9</v>
+        <v>1.6</v>
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>87</v>
       </c>
@@ -1902,21 +1903,21 @@
         <v>88</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E49" s="15">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F49" s="15">
-        <v>1</v>
+        <v>2.9</v>
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="17"/>
     </row>
-    <row r="50" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>87</v>
       </c>
@@ -1924,41 +1925,43 @@
         <v>88</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E50" s="15">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F50" s="15">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="14">
-        <v>4589</v>
+      <c r="C51" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="E51" s="15">
         <v>1.5</v>
       </c>
-      <c r="F51" s="15"/>
+      <c r="F51" s="15">
+        <v>0.7</v>
+      </c>
       <c r="G51" s="16"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>87</v>
       </c>
@@ -1966,19 +1969,19 @@
         <v>88</v>
       </c>
       <c r="C52" s="14">
-        <v>4793</v>
+        <v>4589</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E52" s="15">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F52" s="15"/>
       <c r="G52" s="16"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>87</v>
       </c>
@@ -1986,36 +1989,39 @@
         <v>88</v>
       </c>
       <c r="C53" s="14">
-        <v>4730</v>
+        <v>4793</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E53" s="15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F53" s="15"/>
       <c r="G53" s="16"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="6">
-        <v>421</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C54" s="6">
-        <v>4712</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="14">
+        <v>4730</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E54" s="15">
+        <v>6</v>
+      </c>
+      <c r="F54" s="15"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="17"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>421</v>
       </c>
@@ -2023,16 +2029,16 @@
         <v>108</v>
       </c>
       <c r="C55" s="6">
-        <v>4718</v>
+        <v>4712</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E55" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>421</v>
       </c>
@@ -2040,16 +2046,16 @@
         <v>108</v>
       </c>
       <c r="C56" s="6">
-        <v>4713</v>
+        <v>4718</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>421</v>
       </c>
@@ -2057,16 +2063,16 @@
         <v>108</v>
       </c>
       <c r="C57" s="6">
-        <v>4715</v>
+        <v>4713</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E57" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>421</v>
       </c>
@@ -2074,34 +2080,33 @@
         <v>108</v>
       </c>
       <c r="C58" s="6">
-        <v>4721</v>
+        <v>4715</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E58" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="14">
-        <v>450</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C59" s="14">
-        <v>4735</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="E59" s="15">
-        <v>2</v>
-      </c>
-      <c r="F59" s="15"/>
-    </row>
-    <row r="60" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>421</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="6">
+        <v>4721</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
         <v>450</v>
       </c>
@@ -2109,17 +2114,17 @@
         <v>114</v>
       </c>
       <c r="C60" s="14">
-        <v>4239</v>
+        <v>4735</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E60" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
         <v>450</v>
       </c>
@@ -2127,17 +2132,17 @@
         <v>114</v>
       </c>
       <c r="C61" s="14">
-        <v>4734</v>
+        <v>4239</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E61" s="15">
         <v>3</v>
       </c>
       <c r="F61" s="15"/>
     </row>
-    <row r="62" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
         <v>450</v>
       </c>
@@ -2145,17 +2150,17 @@
         <v>114</v>
       </c>
       <c r="C62" s="14">
-        <v>4720</v>
+        <v>4734</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E62" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F62" s="15"/>
     </row>
-    <row r="63" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
         <v>450</v>
       </c>
@@ -2163,17 +2168,17 @@
         <v>114</v>
       </c>
       <c r="C63" s="14">
-        <v>4731</v>
+        <v>4720</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E63" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F63" s="15"/>
     </row>
-    <row r="64" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
         <v>450</v>
       </c>
@@ -2181,17 +2186,17 @@
         <v>114</v>
       </c>
       <c r="C64" s="14">
-        <v>4585</v>
+        <v>4731</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E64" s="15">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="F64" s="15"/>
     </row>
-    <row r="65" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
         <v>450</v>
       </c>
@@ -2199,17 +2204,17 @@
         <v>114</v>
       </c>
       <c r="C65" s="14">
-        <v>4733</v>
+        <v>4585</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E65" s="15">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
         <v>450</v>
       </c>
@@ -2217,51 +2222,52 @@
         <v>114</v>
       </c>
       <c r="C66" s="14">
+        <v>4733</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E66" s="15">
+        <v>3</v>
+      </c>
+      <c r="F66" s="15"/>
+    </row>
+    <row r="67" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>450</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" s="14">
         <v>4732</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D67" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E67" s="15">
         <v>1.5</v>
       </c>
-      <c r="F66" s="15"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="6">
-        <v>451</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C67" s="6">
-        <v>4740</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E67" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F67" s="15"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>451</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="6" t="s">
         <v>119</v>
       </c>
       <c r="C68" s="6">
-        <v>4737</v>
+        <v>4740</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E68" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>451</v>
       </c>
@@ -2269,57 +2275,74 @@
         <v>119</v>
       </c>
       <c r="C69" s="6">
-        <v>4738</v>
+        <v>4737</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E69" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>451</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="8" t="s">
         <v>119</v>
       </c>
       <c r="C70" s="6">
+        <v>4738</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E70" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>451</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" s="6">
         <v>4736</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D71" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E70" s="5">
+      <c r="E71" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A75" s="19"/>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-    </row>
-    <row r="76" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B76" s="19" t="s">
-        <v>127</v>
-      </c>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="19"/>
+      <c r="B76" s="19"/>
       <c r="C76" s="19"/>
       <c r="D76" s="19"/>
-      <c r="E76" s="5">
-        <f>SUM(E5:E70)</f>
-        <v>140.5</v>
-      </c>
-      <c r="F76" s="5">
-        <f>SUM(F5:F70)</f>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="5">
+        <f>SUM(E5:E71)</f>
+        <v>142.5</v>
+      </c>
+      <c r="F77" s="5">
+        <f>SUM(F5:F71)</f>
         <v>101.50000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="B77:D77"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2334,6 +2357,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100659A167D4CC5EC438DE9848E11CBEA3F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b214d0967801b5c4681ff9774ab7b4fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7a535a6-dfd7-4199-be2a-842d35677326" xmlns:ns4="b1af40a2-86c1-4bae-9fd5-ad1d161ccb8d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ba29263248737a5ec68c1b9165b2e49" ns3:_="" ns4:_="">
     <xsd:import namespace="b7a535a6-dfd7-4199-be2a-842d35677326"/>
@@ -2556,15 +2588,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11FB2DEE-0B14-4095-888E-5BA73ECE0B4D}">
   <ds:schemaRefs>
@@ -2583,6 +2606,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{631E28D5-CD26-42A3-901C-27469E6CABF1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB27589-92E7-461D-B68C-D866F96320FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2599,12 +2630,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{631E28D5-CD26-42A3-901C-27469E6CABF1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add time to excel spreadsheet for tasks #story[421]
</commit_message>
<xml_diff>
--- a/sprint6EstimatedTimes.xlsx
+++ b/sprint6EstimatedTimes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\games\Documents\2020\SENG302\SENG302 Project\team-600\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebek\OneDrive - University of Canterbury\SENG302\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1E1B6-7865-461E-BB0F-F3E0698B5857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="8_{10430196-5930-4A8F-8551-13C767A65B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FD3EF8C-517D-47AA-96F8-D994992E8D46}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="368" windowWidth="22305" windowHeight="7747" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agilefant Timesheet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="132">
   <si>
     <t>Story Id</t>
   </si>
@@ -426,9 +426,6 @@
   </si>
   <si>
     <t>Manually moving a pin to the location you want, will enter an address in the textbox.</t>
-  </si>
-  <si>
-    <t>Fix display issues on Front- End UI</t>
   </si>
 </sst>
 </file>
@@ -849,26 +846,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="104.77734375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.3984375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="33.86328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="104.796875" style="6" customWidth="1"/>
     <col min="5" max="5" width="16" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.73046875" style="5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="19.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -890,7 +887,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>101</v>
       </c>
@@ -910,7 +907,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>101</v>
       </c>
@@ -932,7 +929,7 @@
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="13" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>101</v>
       </c>
@@ -954,7 +951,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>101</v>
       </c>
@@ -976,7 +973,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="17"/>
     </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>101</v>
       </c>
@@ -998,7 +995,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>101</v>
       </c>
@@ -1020,7 +1017,7 @@
       <c r="G7" s="16"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>101</v>
       </c>
@@ -1042,7 +1039,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
     </row>
-    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>101</v>
       </c>
@@ -1064,7 +1061,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>101</v>
       </c>
@@ -1086,7 +1083,7 @@
       <c r="G10" s="16"/>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>101</v>
       </c>
@@ -1108,7 +1105,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1130,7 +1127,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1152,7 +1149,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -1174,7 +1171,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -1193,7 +1190,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1212,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -1237,7 +1234,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
         <v>422</v>
       </c>
@@ -1259,7 +1256,7 @@
       <c r="G18" s="16"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>35</v>
       </c>
@@ -1281,7 +1278,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>35</v>
       </c>
@@ -1303,7 +1300,7 @@
       <c r="G20" s="16"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -1323,7 +1320,7 @@
       <c r="G21" s="16"/>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>35</v>
       </c>
@@ -1343,7 +1340,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>35</v>
       </c>
@@ -1365,7 +1362,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
         <v>35</v>
       </c>
@@ -1387,7 +1384,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
         <v>35</v>
       </c>
@@ -1409,7 +1406,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="17"/>
     </row>
-    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>35</v>
       </c>
@@ -1431,7 +1428,7 @@
       <c r="G26" s="16"/>
       <c r="H26" s="17"/>
     </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>35</v>
       </c>
@@ -1453,7 +1450,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>35</v>
       </c>
@@ -1473,7 +1470,7 @@
       <c r="G28" s="16"/>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
@@ -1493,7 +1490,7 @@
       <c r="G29" s="16"/>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>35</v>
       </c>
@@ -1515,7 +1512,7 @@
       <c r="G30" s="16"/>
       <c r="H30" s="17"/>
     </row>
-    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
         <v>422</v>
       </c>
@@ -1535,7 +1532,7 @@
       <c r="G31" s="16"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>35</v>
       </c>
@@ -1557,27 +1554,26 @@
       <c r="G32" s="16"/>
       <c r="H32" s="17"/>
     </row>
-    <row r="33" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
-        <v>422</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="14">
-        <v>4952</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="5">
         <v>2</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="1"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>63</v>
       </c>
@@ -1585,59 +1581,59 @@
         <v>64</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E34" s="5">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>63</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="6">
+        <v>420</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>67</v>
+      <c r="C35" s="6">
+        <v>4591</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="E35" s="5">
         <v>1.5</v>
       </c>
+      <c r="F35" s="5">
+        <v>0</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>420</v>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="6">
-        <v>4591</v>
+      <c r="C36" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="E36" s="5">
         <v>1.5</v>
       </c>
-      <c r="F36" s="5">
-        <v>0</v>
-      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
@@ -1645,18 +1641,21 @@
         <v>64</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E37" s="5">
-        <v>1.5</v>
+        <v>2.5</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1.3</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>63</v>
       </c>
@@ -1664,21 +1663,21 @@
         <v>64</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E38" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F38" s="5">
-        <v>1.3</v>
+        <v>4.5</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>63</v>
       </c>
@@ -1686,21 +1685,21 @@
         <v>64</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E39" s="5">
         <v>3</v>
       </c>
       <c r="F39" s="5">
-        <v>4.5</v>
+        <v>10.4</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>63</v>
       </c>
@@ -1708,21 +1707,21 @@
         <v>64</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E40" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F40" s="5">
-        <v>10.4</v>
+        <v>0.8</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>63</v>
       </c>
@@ -1730,21 +1729,18 @@
         <v>64</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E41" s="5">
-        <v>1</v>
-      </c>
-      <c r="F41" s="5">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>63</v>
       </c>
@@ -1752,18 +1748,21 @@
         <v>64</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E42" s="5">
-        <v>0.5</v>
+        <v>2.5</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1.2</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>63</v>
       </c>
@@ -1771,21 +1770,21 @@
         <v>64</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E43" s="5">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F43" s="5">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>63</v>
       </c>
@@ -1793,43 +1792,43 @@
         <v>64</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
       </c>
       <c r="F44" s="5">
-        <v>1.8</v>
+        <v>0.5</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="5">
-        <v>2</v>
-      </c>
-      <c r="F45" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F45" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="17"/>
+    </row>
+    <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
         <v>87</v>
       </c>
@@ -1837,21 +1836,21 @@
         <v>88</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E46" s="15">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F46" s="15">
-        <v>1.1000000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
         <v>87</v>
       </c>
@@ -1859,21 +1858,21 @@
         <v>88</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E47" s="15">
         <v>3</v>
       </c>
       <c r="F47" s="15">
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="17"/>
     </row>
-    <row r="48" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
         <v>87</v>
       </c>
@@ -1881,21 +1880,21 @@
         <v>88</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E48" s="15">
         <v>3</v>
       </c>
       <c r="F48" s="15">
-        <v>1.6</v>
+        <v>2.9</v>
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="14" t="s">
         <v>87</v>
       </c>
@@ -1903,21 +1902,21 @@
         <v>88</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E49" s="15">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F49" s="15">
-        <v>2.9</v>
+        <v>1</v>
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="17"/>
     </row>
-    <row r="50" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>87</v>
       </c>
@@ -1925,43 +1924,41 @@
         <v>88</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E50" s="15">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="F50" s="15">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="14" t="s">
-        <v>91</v>
+      <c r="C51" s="14">
+        <v>4589</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="E51" s="15">
         <v>1.5</v>
       </c>
-      <c r="F51" s="15">
-        <v>0.7</v>
-      </c>
+      <c r="F51" s="15"/>
       <c r="G51" s="16"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="14" t="s">
         <v>87</v>
       </c>
@@ -1969,19 +1966,19 @@
         <v>88</v>
       </c>
       <c r="C52" s="14">
-        <v>4589</v>
+        <v>4793</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E52" s="15">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F52" s="15"/>
       <c r="G52" s="16"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
         <v>87</v>
       </c>
@@ -1989,39 +1986,36 @@
         <v>88</v>
       </c>
       <c r="C53" s="14">
-        <v>4793</v>
+        <v>4730</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E53" s="15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F53" s="15"/>
       <c r="G53" s="16"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" s="14">
-        <v>4730</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E54" s="15">
-        <v>6</v>
-      </c>
-      <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="6">
+        <v>421</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="6">
+        <v>4712</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>421</v>
       </c>
@@ -2029,16 +2023,19 @@
         <v>108</v>
       </c>
       <c r="C55" s="6">
-        <v>4712</v>
+        <v>4718</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E55" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F55" s="5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>421</v>
       </c>
@@ -2046,16 +2043,16 @@
         <v>108</v>
       </c>
       <c r="C56" s="6">
-        <v>4718</v>
+        <v>4713</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>421</v>
       </c>
@@ -2063,16 +2060,16 @@
         <v>108</v>
       </c>
       <c r="C57" s="6">
-        <v>4713</v>
+        <v>4715</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E57" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>421</v>
       </c>
@@ -2080,33 +2077,34 @@
         <v>108</v>
       </c>
       <c r="C58" s="6">
-        <v>4715</v>
+        <v>4721</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E58" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="6">
-        <v>421</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" s="6">
-        <v>4721</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E59" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="14">
+        <v>450</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="14">
+        <v>4735</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="15">
+        <v>2</v>
+      </c>
+      <c r="F59" s="15"/>
+    </row>
+    <row r="60" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="14">
         <v>450</v>
       </c>
@@ -2114,17 +2112,17 @@
         <v>114</v>
       </c>
       <c r="C60" s="14">
-        <v>4735</v>
+        <v>4239</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E60" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="14">
         <v>450</v>
       </c>
@@ -2132,17 +2130,17 @@
         <v>114</v>
       </c>
       <c r="C61" s="14">
-        <v>4239</v>
+        <v>4734</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E61" s="15">
         <v>3</v>
       </c>
       <c r="F61" s="15"/>
     </row>
-    <row r="62" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="14">
         <v>450</v>
       </c>
@@ -2150,17 +2148,17 @@
         <v>114</v>
       </c>
       <c r="C62" s="14">
-        <v>4734</v>
+        <v>4720</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E62" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F62" s="15"/>
     </row>
-    <row r="63" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="14">
         <v>450</v>
       </c>
@@ -2168,17 +2166,17 @@
         <v>114</v>
       </c>
       <c r="C63" s="14">
-        <v>4720</v>
+        <v>4731</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E63" s="15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F63" s="15"/>
     </row>
-    <row r="64" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="14">
         <v>450</v>
       </c>
@@ -2186,17 +2184,17 @@
         <v>114</v>
       </c>
       <c r="C64" s="14">
-        <v>4731</v>
+        <v>4585</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E64" s="15">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="F64" s="15"/>
     </row>
-    <row r="65" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14">
         <v>450</v>
       </c>
@@ -2204,17 +2202,17 @@
         <v>114</v>
       </c>
       <c r="C65" s="14">
-        <v>4585</v>
+        <v>4733</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E65" s="15">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="14">
         <v>450</v>
       </c>
@@ -2222,52 +2220,51 @@
         <v>114</v>
       </c>
       <c r="C66" s="14">
-        <v>4733</v>
+        <v>4732</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E66" s="15">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="F66" s="15"/>
     </row>
-    <row r="67" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="14">
-        <v>450</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C67" s="14">
-        <v>4732</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E67" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="F67" s="15"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="6">
+        <v>451</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="6">
+        <v>4740</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>451</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="8" t="s">
         <v>119</v>
       </c>
       <c r="C68" s="6">
-        <v>4740</v>
+        <v>4737</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E68" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
         <v>451</v>
       </c>
@@ -2275,74 +2272,57 @@
         <v>119</v>
       </c>
       <c r="C69" s="6">
-        <v>4737</v>
+        <v>4738</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E69" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
         <v>451</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="9" t="s">
         <v>119</v>
       </c>
       <c r="C70" s="6">
-        <v>4738</v>
+        <v>4736</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E70" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="6">
-        <v>451</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C71" s="6">
-        <v>4736</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E71" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="19"/>
-      <c r="B76" s="19"/>
+    <row r="75" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+    </row>
+    <row r="76" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B76" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="C76" s="19"/>
       <c r="D76" s="19"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19"/>
-      <c r="E77" s="5">
-        <f>SUM(E5:E71)</f>
-        <v>142.5</v>
-      </c>
-      <c r="F77" s="5">
-        <f>SUM(F5:F71)</f>
-        <v>101.50000000000001</v>
+      <c r="E76" s="5">
+        <f>SUM(E5:E70)</f>
+        <v>140.5</v>
+      </c>
+      <c r="F76" s="5">
+        <f>SUM(F5:F70)</f>
+        <v>103.60000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="B76:D76"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated user response to use a dedicated location response #story[419]
</commit_message>
<xml_diff>
--- a/sprint6EstimatedTimes.xlsx
+++ b/sprint6EstimatedTimes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\games\Documents\2020\SENG302\SENG302 Project\team-600\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UC300\SENG302\team-600\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1E1B6-7865-461E-BB0F-F3E0698B5857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAB326B-047B-4BEC-8F77-0AA03CEC00E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agilefant Timesheet" sheetId="1" r:id="rId1"/>
@@ -852,8 +852,8 @@
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1695,7 +1695,7 @@
         <v>3</v>
       </c>
       <c r="F39" s="5">
-        <v>4.5</v>
+        <v>21</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
@@ -1977,7 +1977,9 @@
       <c r="E52" s="15">
         <v>1.5</v>
       </c>
-      <c r="F52" s="15"/>
+      <c r="F52" s="15">
+        <v>6.4</v>
+      </c>
       <c r="G52" s="16"/>
       <c r="H52" s="17"/>
     </row>
@@ -2336,7 +2338,7 @@
       </c>
       <c r="F77" s="5">
         <f>SUM(F5:F71)</f>
-        <v>101.50000000000001</v>
+        <v>124.40000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -2357,15 +2359,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100659A167D4CC5EC438DE9848E11CBEA3F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b214d0967801b5c4681ff9774ab7b4fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7a535a6-dfd7-4199-be2a-842d35677326" xmlns:ns4="b1af40a2-86c1-4bae-9fd5-ad1d161ccb8d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ba29263248737a5ec68c1b9165b2e49" ns3:_="" ns4:_="">
     <xsd:import namespace="b7a535a6-dfd7-4199-be2a-842d35677326"/>
@@ -2588,6 +2581,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11FB2DEE-0B14-4095-888E-5BA73ECE0B4D}">
   <ds:schemaRefs>
@@ -2606,14 +2608,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{631E28D5-CD26-42A3-901C-27469E6CABF1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB27589-92E7-461D-B68C-D866F96320FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2630,4 +2624,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{631E28D5-CD26-42A3-901C-27469E6CABF1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>